<commit_message>
Added analysis data of 10 repos and updated repo list
</commit_message>
<xml_diff>
--- a/SENG300 Group 12 Repositories.xlsx
+++ b/SENG300 Group 12 Repositories.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t>Repository Name</t>
   </si>
@@ -350,6 +350,126 @@
   </si>
   <si>
     <t>https://github.com/bootique/bootique</t>
+  </si>
+  <si>
+    <t>Terasology</t>
+  </si>
+  <si>
+    <t>https://github.com/MovingBlocks/Terasology</t>
+  </si>
+  <si>
+    <t>JOE</t>
+  </si>
+  <si>
+    <t>https://github.com/joekoolade/JOE</t>
+  </si>
+  <si>
+    <t>RestApiUsingSpringBoot</t>
+  </si>
+  <si>
+    <t>https://github.com/smartudhaya/RestApiUsingSpringBoot</t>
+  </si>
+  <si>
+    <t>TastefulChoiceSelections</t>
+  </si>
+  <si>
+    <t>https://github.com/Matmatix/TastefulChoiceSelections</t>
+  </si>
+  <si>
+    <t>minijax</t>
+  </si>
+  <si>
+    <t>https://github.com/minijax/minijax</t>
+  </si>
+  <si>
+    <t>aws-doc-sdk-examples</t>
+  </si>
+  <si>
+    <t>https://github.com/awsdocs/aws-doc-sdk-examples</t>
+  </si>
+  <si>
+    <t>buck</t>
+  </si>
+  <si>
+    <t>https://github.com/facebook/buck</t>
+  </si>
+  <si>
+    <t>lwhtarena_note</t>
+  </si>
+  <si>
+    <t>https://github.com/LWHTarena/lwhtarena_note</t>
+  </si>
+  <si>
+    <t>mdw</t>
+  </si>
+  <si>
+    <t>https://github.com/CenturyLinkCloud/mdw</t>
+  </si>
+  <si>
+    <t>etecJarra</t>
+  </si>
+  <si>
+    <t>https://github.com/WilkerS1/etecJarra</t>
+  </si>
+  <si>
+    <t>vigilant-eureka</t>
+  </si>
+  <si>
+    <t>https://github.com/dubeboy/vigilant-eureka</t>
+  </si>
+  <si>
+    <t>tink</t>
+  </si>
+  <si>
+    <t>https://github.com/google/tink</t>
+  </si>
+  <si>
+    <t>KindleQuickFormatter</t>
+  </si>
+  <si>
+    <t>https://github.com/echomap/KindleQuickFormatter</t>
+  </si>
+  <si>
+    <t>PhantomBot</t>
+  </si>
+  <si>
+    <t>https://github.com/PhantomBot/PhantomBot</t>
+  </si>
+  <si>
+    <t>KaellyBot</t>
+  </si>
+  <si>
+    <t>https://github.com/Kaysoro/KaellyBot</t>
+  </si>
+  <si>
+    <t>bndtools</t>
+  </si>
+  <si>
+    <t>https://github.com/bndtools/bndtools</t>
+  </si>
+  <si>
+    <t>presto</t>
+  </si>
+  <si>
+    <t>https://github.com/starburstdata/presto</t>
+  </si>
+  <si>
+    <t>pepsimod</t>
+  </si>
+  <si>
+    <t>https://github.com/Team-Pepsi/pepsimod</t>
+  </si>
+  <si>
+    <t>kanzi</t>
+  </si>
+  <si>
+    <t>https://github.com/flanglet/kanzi</t>
+  </si>
+  <si>
+    <t>pong-or-something</t>
+  </si>
+  <si>
+    <t>https://github.com/ethanlosten/pong-or-something</t>
   </si>
 </sst>
 </file>
@@ -407,7 +527,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
@@ -863,6 +986,166 @@
       </c>
       <c r="B55" s="2" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +1204,27 @@
     <hyperlink r:id="rId52" ref="B53"/>
     <hyperlink r:id="rId53" ref="B54"/>
     <hyperlink r:id="rId54" ref="B55"/>
+    <hyperlink r:id="rId55" ref="B56"/>
+    <hyperlink r:id="rId56" ref="B57"/>
+    <hyperlink r:id="rId57" ref="B58"/>
+    <hyperlink r:id="rId58" ref="B59"/>
+    <hyperlink r:id="rId59" ref="B60"/>
+    <hyperlink r:id="rId60" ref="B61"/>
+    <hyperlink r:id="rId61" ref="B62"/>
+    <hyperlink r:id="rId62" ref="B63"/>
+    <hyperlink r:id="rId63" ref="B64"/>
+    <hyperlink r:id="rId64" ref="B65"/>
+    <hyperlink r:id="rId65" ref="B66"/>
+    <hyperlink r:id="rId66" ref="B67"/>
+    <hyperlink r:id="rId67" ref="B68"/>
+    <hyperlink r:id="rId68" ref="B69"/>
+    <hyperlink r:id="rId69" ref="B70"/>
+    <hyperlink r:id="rId70" ref="B71"/>
+    <hyperlink r:id="rId71" ref="B72"/>
+    <hyperlink r:id="rId72" ref="B73"/>
+    <hyperlink r:id="rId73" ref="B74"/>
+    <hyperlink r:id="rId74" ref="B75"/>
   </hyperlinks>
-  <drawing r:id="rId55"/>
+  <drawing r:id="rId75"/>
 </worksheet>
 </file>
</xml_diff>